<commit_message>
Fixed typo in list, peache -> peach
</commit_message>
<xml_diff>
--- a/RandomData/inventory.xlsx
+++ b/RandomData/inventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11760" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="zehrs" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="898">
   <si>
     <t>coca_cola 350</t>
   </si>
@@ -1131,9 +1131,6 @@
     <t>yellow_plum 499</t>
   </si>
   <si>
-    <t>peache 499</t>
-  </si>
-  <si>
     <t>crab_claw 4399</t>
   </si>
   <si>
@@ -1305,9 +1302,6 @@
     <t>grape 148</t>
   </si>
   <si>
-    <t>peache 334</t>
-  </si>
-  <si>
     <t>green_bean 198</t>
   </si>
   <si>
@@ -1506,9 +1500,6 @@
     <t>tortilla_chip 299</t>
   </si>
   <si>
-    <t>peache 288</t>
-  </si>
-  <si>
     <t>cookie 199</t>
   </si>
   <si>
@@ -2406,9 +2397,6 @@
     <t>pc_tortilla_chip</t>
   </si>
   <si>
-    <t>peache</t>
-  </si>
-  <si>
     <t>peanut</t>
   </si>
   <si>
@@ -2713,6 +2701,21 @@
   </si>
   <si>
     <t>zucchini</t>
+  </si>
+  <si>
+    <t>RANDBETWEEN(1,305)</t>
+  </si>
+  <si>
+    <t>peach 499</t>
+  </si>
+  <si>
+    <t>peach 334</t>
+  </si>
+  <si>
+    <t>peach 288</t>
+  </si>
+  <si>
+    <t>peach</t>
   </si>
 </sst>
 </file>
@@ -3025,8 +3028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="E1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3046,12 +3049,12 @@
     </row>
     <row r="3" spans="5:5">
       <c r="E3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="4" spans="5:5">
       <c r="E4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="5" spans="5:5">
@@ -3061,12 +3064,12 @@
     </row>
     <row r="6" spans="5:5">
       <c r="E6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" spans="5:5">
       <c r="E7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" spans="5:5">
@@ -3106,7 +3109,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="16" spans="5:5">
@@ -3140,8 +3143,8 @@
       </c>
     </row>
     <row r="22" spans="5:5">
-      <c r="E22" t="s">
-        <v>369</v>
+      <c r="E22" s="1" t="s">
+        <v>894</v>
       </c>
     </row>
     <row r="23" spans="5:5">
@@ -3151,7 +3154,7 @@
     </row>
     <row r="24" spans="5:5">
       <c r="E24" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="25" spans="5:5">
@@ -3161,7 +3164,7 @@
     </row>
     <row r="26" spans="5:5">
       <c r="E26" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="27" spans="5:5">
@@ -3181,7 +3184,7 @@
     </row>
     <row r="30" spans="5:5">
       <c r="E30" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="31" spans="5:5">
@@ -3191,7 +3194,7 @@
     </row>
     <row r="32" spans="5:5">
       <c r="E32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="33" spans="5:5">
@@ -3241,12 +3244,12 @@
     </row>
     <row r="42" spans="5:5">
       <c r="E42" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="43" spans="5:5">
       <c r="E43" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="44" spans="5:5">
@@ -3276,7 +3279,7 @@
     </row>
     <row r="49" spans="5:5">
       <c r="E49" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="50" spans="5:5">
@@ -3286,22 +3289,22 @@
     </row>
     <row r="51" spans="5:5">
       <c r="E51" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="52" spans="5:5">
       <c r="E52" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="53" spans="5:5">
       <c r="E53" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="54" spans="5:5">
       <c r="E54" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="55" spans="5:5">
@@ -3326,7 +3329,7 @@
     </row>
     <row r="59" spans="5:5">
       <c r="E59" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="60" spans="5:5">
@@ -3346,22 +3349,22 @@
     </row>
     <row r="63" spans="5:5">
       <c r="E63" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="64" spans="5:5">
       <c r="E64" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="65" spans="5:5">
       <c r="E65" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="66" spans="5:5">
       <c r="E66" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="67" spans="5:5">
@@ -3381,7 +3384,7 @@
     </row>
     <row r="70" spans="5:5">
       <c r="E70" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="71" spans="5:5">
@@ -3391,12 +3394,12 @@
     </row>
     <row r="72" spans="5:5">
       <c r="E72" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="73" spans="5:5">
       <c r="E73" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="74" spans="5:5">
@@ -3411,7 +3414,7 @@
     </row>
     <row r="76" spans="5:5">
       <c r="E76" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="77" spans="5:5">
@@ -3426,7 +3429,7 @@
     </row>
     <row r="79" spans="5:5">
       <c r="E79" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="80" spans="5:5">
@@ -3436,42 +3439,42 @@
     </row>
     <row r="81" spans="5:5">
       <c r="E81" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="89" spans="5:5">
@@ -3481,7 +3484,7 @@
     </row>
     <row r="90" spans="5:5">
       <c r="E90" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="91" spans="5:5">
@@ -3491,7 +3494,7 @@
     </row>
     <row r="92" spans="5:5">
       <c r="E92" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="93" spans="5:5">
@@ -3516,17 +3519,17 @@
     </row>
     <row r="97" spans="5:5">
       <c r="E97" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="100" spans="5:5">
@@ -3536,22 +3539,22 @@
     </row>
     <row r="101" spans="5:5">
       <c r="E101" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="105" spans="5:5">
@@ -3576,7 +3579,7 @@
     </row>
     <row r="109" spans="5:5">
       <c r="E109" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="110" spans="5:5">
@@ -3586,12 +3589,12 @@
     </row>
     <row r="111" spans="5:5">
       <c r="E111" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="113" spans="5:5">
@@ -3621,7 +3624,7 @@
     </row>
     <row r="118" spans="5:5">
       <c r="E118" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="119" spans="5:5">
@@ -3631,7 +3634,7 @@
     </row>
     <row r="120" spans="5:5">
       <c r="E120" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="121" spans="5:5">
@@ -3641,7 +3644,7 @@
     </row>
     <row r="122" spans="5:5">
       <c r="E122" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="123" spans="5:5">
@@ -3651,7 +3654,7 @@
     </row>
     <row r="124" spans="5:5">
       <c r="E124" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="125" spans="5:5">
@@ -3661,37 +3664,37 @@
     </row>
     <row r="126" spans="5:5">
       <c r="E126" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="127" spans="5:5">
       <c r="E127" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="128" spans="5:5">
       <c r="E128" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="129" spans="5:5">
       <c r="E129" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="130" spans="5:5">
       <c r="E130" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="131" spans="5:5">
       <c r="E131" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="132" spans="5:5">
       <c r="E132" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="133" spans="5:5">
@@ -3711,7 +3714,7 @@
     </row>
     <row r="136" spans="5:5">
       <c r="E136" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="137" spans="5:5">
@@ -3746,17 +3749,17 @@
     </row>
     <row r="143" spans="5:5">
       <c r="E143" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="144" spans="5:5">
       <c r="E144" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="145" spans="5:5">
       <c r="E145" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="146" spans="5:5">
@@ -3766,7 +3769,7 @@
     </row>
     <row r="147" spans="5:5">
       <c r="E147" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="148" spans="5:5">
@@ -3786,12 +3789,12 @@
     </row>
     <row r="151" spans="5:5">
       <c r="E151" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="152" spans="5:5">
       <c r="E152" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="153" spans="5:5">
@@ -3806,27 +3809,27 @@
     </row>
     <row r="155" spans="5:5">
       <c r="E155" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="156" spans="5:5">
       <c r="E156" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="157" spans="5:5">
       <c r="E157" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="158" spans="5:5">
       <c r="E158" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="159" spans="5:5">
       <c r="E159" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="160" spans="5:5">
@@ -3848,35 +3851,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="E1:E55"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E31" sqref="E1:E1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="5:5">
       <c r="E1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2" spans="5:5">
       <c r="E2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3" spans="5:5">
       <c r="E3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4" spans="5:5">
       <c r="E4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="5:5">
       <c r="E5" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="6" spans="5:5">
@@ -3886,7 +3889,7 @@
     </row>
     <row r="7" spans="5:5">
       <c r="E7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="8" spans="5:5">
@@ -3901,12 +3904,12 @@
     </row>
     <row r="10" spans="5:5">
       <c r="E10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="5:5">
       <c r="E11" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="12" spans="5:5">
@@ -3916,7 +3919,7 @@
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -3926,7 +3929,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="16" spans="5:5">
@@ -3936,7 +3939,7 @@
     </row>
     <row r="17" spans="5:5">
       <c r="E17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="18" spans="5:5">
@@ -3946,7 +3949,7 @@
     </row>
     <row r="19" spans="5:5">
       <c r="E19" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="20" spans="5:5">
@@ -3956,12 +3959,12 @@
     </row>
     <row r="21" spans="5:5">
       <c r="E21" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="22" spans="5:5">
       <c r="E22" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="23" spans="5:5">
@@ -3986,17 +3989,17 @@
     </row>
     <row r="27" spans="5:5">
       <c r="E27" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="28" spans="5:5">
       <c r="E28" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="29" spans="5:5">
       <c r="E29" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="30" spans="5:5">
@@ -4016,7 +4019,7 @@
     </row>
     <row r="33" spans="5:5">
       <c r="E33" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="34" spans="5:5">
@@ -4071,7 +4074,7 @@
     </row>
     <row r="44" spans="5:5">
       <c r="E44" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="45" spans="5:5">
@@ -4081,12 +4084,12 @@
     </row>
     <row r="46" spans="5:5">
       <c r="E46" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="47" spans="5:5">
       <c r="E47" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="48" spans="5:5">
@@ -4096,7 +4099,7 @@
     </row>
     <row r="49" spans="5:5">
       <c r="E49" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="50" spans="5:5">
@@ -4111,7 +4114,7 @@
     </row>
     <row r="52" spans="5:5">
       <c r="E52" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="53" spans="5:5">
@@ -4126,7 +4129,7 @@
     </row>
     <row r="55" spans="5:5">
       <c r="E55" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
   </sheetData>
@@ -4138,8 +4141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D1:D100"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D28" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4161,7 +4164,7 @@
     </row>
     <row r="4" spans="4:4">
       <c r="D4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="5" spans="4:4">
@@ -4185,28 +4188,28 @@
       </c>
     </row>
     <row r="9" spans="4:4">
-      <c r="D9" t="s">
-        <v>427</v>
+      <c r="D9" s="1" t="s">
+        <v>895</v>
       </c>
     </row>
     <row r="10" spans="4:4">
       <c r="D10" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="11" spans="4:4">
       <c r="D11" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="12" spans="4:4">
       <c r="D12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="13" spans="4:4">
       <c r="D13" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="14" spans="4:4">
@@ -4216,7 +4219,7 @@
     </row>
     <row r="15" spans="4:4">
       <c r="D15" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="16" spans="4:4">
@@ -4226,7 +4229,7 @@
     </row>
     <row r="17" spans="4:4">
       <c r="D17" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="18" spans="4:4">
@@ -4236,12 +4239,12 @@
     </row>
     <row r="19" spans="4:4">
       <c r="D19" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="20" spans="4:4">
       <c r="D20" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="21" spans="4:4">
@@ -4266,12 +4269,12 @@
     </row>
     <row r="25" spans="4:4">
       <c r="D25" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="26" spans="4:4">
       <c r="D26" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="27" spans="4:4">
@@ -4301,7 +4304,7 @@
     </row>
     <row r="32" spans="4:4">
       <c r="D32" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="33" spans="4:4">
@@ -4311,7 +4314,7 @@
     </row>
     <row r="34" spans="4:4">
       <c r="D34" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="35" spans="4:4">
@@ -4341,7 +4344,7 @@
     </row>
     <row r="40" spans="4:4">
       <c r="D40" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="41" spans="4:4">
@@ -4351,22 +4354,22 @@
     </row>
     <row r="42" spans="4:4">
       <c r="D42" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="43" spans="4:4">
       <c r="D43" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="44" spans="4:4">
       <c r="D44" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="45" spans="4:4">
       <c r="D45" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="46" spans="4:4">
@@ -4376,27 +4379,27 @@
     </row>
     <row r="47" spans="4:4">
       <c r="D47" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="48" spans="4:4">
       <c r="D48" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="49" spans="4:4">
       <c r="D49" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="50" spans="4:4">
       <c r="D50" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="51" spans="4:4">
       <c r="D51" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="52" spans="4:4">
@@ -4411,7 +4414,7 @@
     </row>
     <row r="54" spans="4:4">
       <c r="D54" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="55" spans="4:4">
@@ -4426,7 +4429,7 @@
     </row>
     <row r="57" spans="4:4">
       <c r="D57" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="58" spans="4:4">
@@ -4436,7 +4439,7 @@
     </row>
     <row r="59" spans="4:4">
       <c r="D59" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="60" spans="4:4">
@@ -4451,12 +4454,12 @@
     </row>
     <row r="62" spans="4:4">
       <c r="D62" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="63" spans="4:4">
       <c r="D63" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="64" spans="4:4">
@@ -4476,12 +4479,12 @@
     </row>
     <row r="67" spans="4:4">
       <c r="D67" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="68" spans="4:4">
       <c r="D68" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="69" spans="4:4">
@@ -4496,12 +4499,12 @@
     </row>
     <row r="71" spans="4:4">
       <c r="D71" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="72" spans="4:4">
       <c r="D72" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="73" spans="4:4">
@@ -4531,12 +4534,12 @@
     </row>
     <row r="78" spans="4:4">
       <c r="D78" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="79" spans="4:4">
       <c r="D79" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="80" spans="4:4">
@@ -4561,7 +4564,7 @@
     </row>
     <row r="84" spans="4:4">
       <c r="D84" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="85" spans="4:4">
@@ -4591,12 +4594,12 @@
     </row>
     <row r="90" spans="4:4">
       <c r="D90" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="91" spans="4:4">
       <c r="D91" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="92" spans="4:4">
@@ -4636,7 +4639,7 @@
     </row>
     <row r="99" spans="4:4">
       <c r="D99" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="100" spans="4:4">
@@ -4654,7 +4657,7 @@
   <dimension ref="E1:E98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4681,12 +4684,12 @@
     </row>
     <row r="5" spans="5:5">
       <c r="E5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="6" spans="5:5">
       <c r="E6" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="7" spans="5:5">
@@ -4706,7 +4709,7 @@
     </row>
     <row r="10" spans="5:5">
       <c r="E10" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="11" spans="5:5">
@@ -4716,12 +4719,12 @@
     </row>
     <row r="12" spans="5:5">
       <c r="E12" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -4766,17 +4769,17 @@
     </row>
     <row r="22" spans="5:5">
       <c r="E22" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="23" spans="5:5">
       <c r="E23" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="24" spans="5:5">
       <c r="E24" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="25" spans="5:5">
@@ -4836,7 +4839,7 @@
     </row>
     <row r="36" spans="5:5">
       <c r="E36" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="37" spans="5:5">
@@ -4946,22 +4949,22 @@
     </row>
     <row r="58" spans="5:5">
       <c r="E58" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="59" spans="5:5">
       <c r="E59" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="60" spans="5:5">
       <c r="E60" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="61" spans="5:5">
       <c r="E61" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="62" spans="5:5">
@@ -4971,7 +4974,7 @@
     </row>
     <row r="63" spans="5:5">
       <c r="E63" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="64" spans="5:5">
@@ -4981,7 +4984,7 @@
     </row>
     <row r="65" spans="5:5">
       <c r="E65" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="66" spans="5:5">
@@ -5016,7 +5019,7 @@
     </row>
     <row r="72" spans="5:5">
       <c r="E72" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="73" spans="5:5">
@@ -5056,12 +5059,12 @@
     </row>
     <row r="80" spans="5:5">
       <c r="E80" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="82" spans="5:5">
@@ -5101,7 +5104,7 @@
     </row>
     <row r="89" spans="5:5">
       <c r="E89" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="90" spans="5:5">
@@ -5126,7 +5129,7 @@
     </row>
     <row r="94" spans="5:5">
       <c r="E94" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="95" spans="5:5">
@@ -5159,14 +5162,14 @@
   <dimension ref="E1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="5:5">
       <c r="E1" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="2" spans="5:5">
@@ -5181,17 +5184,17 @@
     </row>
     <row r="4" spans="5:5">
       <c r="E4" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="5" spans="5:5">
       <c r="E5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" spans="5:5">
       <c r="E6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" spans="5:5">
@@ -5221,7 +5224,7 @@
     </row>
     <row r="12" spans="5:5">
       <c r="E12" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="13" spans="5:5">
@@ -5231,12 +5234,12 @@
     </row>
     <row r="14" spans="5:5">
       <c r="E14" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="16" spans="5:5">
@@ -5271,17 +5274,17 @@
     </row>
     <row r="22" spans="5:5">
       <c r="E22" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="23" spans="5:5">
       <c r="E23" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="24" spans="5:5">
       <c r="E24" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="25" spans="5:5">
@@ -5301,7 +5304,7 @@
     </row>
     <row r="28" spans="5:5">
       <c r="E28" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="29" spans="5:5">
@@ -5318,8 +5321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="E1:E78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E40" sqref="E1:E1048576"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5346,7 +5349,7 @@
     </row>
     <row r="5" spans="5:5">
       <c r="E5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="6" spans="5:5">
@@ -5361,7 +5364,7 @@
     </row>
     <row r="8" spans="5:5">
       <c r="E8" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="9" spans="5:5">
@@ -5386,12 +5389,12 @@
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="14" spans="5:5">
       <c r="E14" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="15" spans="5:5">
@@ -5406,7 +5409,7 @@
     </row>
     <row r="17" spans="5:5">
       <c r="E17" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="18" spans="5:5">
@@ -5436,17 +5439,17 @@
     </row>
     <row r="23" spans="5:5">
       <c r="E23" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="24" spans="5:5">
       <c r="E24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="25" spans="5:5">
       <c r="E25" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="26" spans="5:5">
@@ -5486,22 +5489,22 @@
     </row>
     <row r="33" spans="5:5">
       <c r="E33" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="34" spans="5:5">
-      <c r="E34" t="s">
-        <v>369</v>
+      <c r="E34" s="1" t="s">
+        <v>894</v>
       </c>
     </row>
     <row r="35" spans="5:5">
       <c r="E35" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="36" spans="5:5">
       <c r="E36" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="37" spans="5:5">
@@ -5526,7 +5529,7 @@
     </row>
     <row r="41" spans="5:5">
       <c r="E41" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="42" spans="5:5">
@@ -5541,7 +5544,7 @@
     </row>
     <row r="44" spans="5:5">
       <c r="E44" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="45" spans="5:5">
@@ -5566,7 +5569,7 @@
     </row>
     <row r="49" spans="5:5">
       <c r="E49" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="50" spans="5:5">
@@ -5586,7 +5589,7 @@
     </row>
     <row r="53" spans="5:5">
       <c r="E53" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="54" spans="5:5">
@@ -5601,7 +5604,7 @@
     </row>
     <row r="56" spans="5:5">
       <c r="E56" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="57" spans="5:5">
@@ -5636,7 +5639,7 @@
     </row>
     <row r="63" spans="5:5">
       <c r="E63" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="64" spans="5:5">
@@ -5656,27 +5659,27 @@
     </row>
     <row r="67" spans="5:5">
       <c r="E67" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="68" spans="5:5">
       <c r="E68" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="69" spans="5:5">
       <c r="E69" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="70" spans="5:5">
       <c r="E70" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="71" spans="5:5">
       <c r="E71" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="72" spans="5:5">
@@ -5686,7 +5689,7 @@
     </row>
     <row r="73" spans="5:5">
       <c r="E73" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="74" spans="5:5">
@@ -5696,7 +5699,7 @@
     </row>
     <row r="75" spans="5:5">
       <c r="E75" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="76" spans="5:5">
@@ -5711,7 +5714,7 @@
     </row>
     <row r="78" spans="5:5">
       <c r="E78" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -5766,7 +5769,7 @@
     </row>
     <row r="8" spans="7:7">
       <c r="G8" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="9" spans="7:7">
@@ -5776,7 +5779,7 @@
     </row>
     <row r="10" spans="7:7">
       <c r="G10" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="11" spans="7:7">
@@ -5786,12 +5789,12 @@
     </row>
     <row r="12" spans="7:7">
       <c r="G12" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="13" spans="7:7">
       <c r="G13" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="14" spans="7:7">
@@ -5816,27 +5819,27 @@
     </row>
     <row r="18" spans="7:7">
       <c r="G18" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="19" spans="7:7">
       <c r="G19" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="20" spans="7:7">
       <c r="G20" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="21" spans="7:7">
       <c r="G21" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="22" spans="7:7">
       <c r="G22" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="23" spans="7:7">
@@ -5846,7 +5849,7 @@
     </row>
     <row r="24" spans="7:7">
       <c r="G24" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="25" spans="7:7">
@@ -5876,7 +5879,7 @@
     </row>
     <row r="30" spans="7:7">
       <c r="G30" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="31" spans="7:7">
@@ -5896,12 +5899,12 @@
     </row>
     <row r="34" spans="7:7">
       <c r="G34" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="35" spans="7:7">
       <c r="G35" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="36" spans="7:7">
@@ -5941,7 +5944,7 @@
     </row>
     <row r="43" spans="7:7">
       <c r="G43" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="44" spans="7:7">
@@ -5956,7 +5959,7 @@
     </row>
     <row r="46" spans="7:7">
       <c r="G46" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="47" spans="7:7">
@@ -5981,12 +5984,12 @@
     </row>
     <row r="51" spans="7:7">
       <c r="G51" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="52" spans="7:7">
       <c r="G52" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="53" spans="7:7">
@@ -6004,14 +6007,14 @@
   <dimension ref="G1:G73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G42" sqref="G1:G1048576"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="7:7">
-      <c r="G1" t="s">
-        <v>494</v>
+      <c r="G1" s="1" t="s">
+        <v>896</v>
       </c>
     </row>
     <row r="2" spans="7:7">
@@ -6031,7 +6034,7 @@
     </row>
     <row r="5" spans="7:7">
       <c r="G5" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="6" spans="7:7">
@@ -6046,7 +6049,7 @@
     </row>
     <row r="8" spans="7:7">
       <c r="G8" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="9" spans="7:7">
@@ -6056,7 +6059,7 @@
     </row>
     <row r="10" spans="7:7">
       <c r="G10" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="11" spans="7:7">
@@ -6066,17 +6069,17 @@
     </row>
     <row r="12" spans="7:7">
       <c r="G12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="13" spans="7:7">
       <c r="G13" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="14" spans="7:7">
       <c r="G14" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="15" spans="7:7">
@@ -6086,7 +6089,7 @@
     </row>
     <row r="16" spans="7:7">
       <c r="G16" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="17" spans="7:7">
@@ -6096,17 +6099,17 @@
     </row>
     <row r="18" spans="7:7">
       <c r="G18" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="19" spans="7:7">
       <c r="G19" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="20" spans="7:7">
       <c r="G20" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="21" spans="7:7">
@@ -6116,7 +6119,7 @@
     </row>
     <row r="22" spans="7:7">
       <c r="G22" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="23" spans="7:7">
@@ -6136,17 +6139,17 @@
     </row>
     <row r="26" spans="7:7">
       <c r="G26" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="27" spans="7:7">
       <c r="G27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="28" spans="7:7">
       <c r="G28" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="29" spans="7:7">
@@ -6161,7 +6164,7 @@
     </row>
     <row r="31" spans="7:7">
       <c r="G31" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="32" spans="7:7">
@@ -6171,12 +6174,12 @@
     </row>
     <row r="33" spans="7:7">
       <c r="G33" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="34" spans="7:7">
       <c r="G34" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="35" spans="7:7">
@@ -6186,7 +6189,7 @@
     </row>
     <row r="36" spans="7:7">
       <c r="G36" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="37" spans="7:7">
@@ -6211,7 +6214,7 @@
     </row>
     <row r="41" spans="7:7">
       <c r="G41" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="42" spans="7:7">
@@ -6221,7 +6224,7 @@
     </row>
     <row r="43" spans="7:7">
       <c r="G43" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="44" spans="7:7">
@@ -6236,17 +6239,17 @@
     </row>
     <row r="46" spans="7:7">
       <c r="G46" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="47" spans="7:7">
       <c r="G47" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="48" spans="7:7">
       <c r="G48" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="49" spans="7:7">
@@ -6266,7 +6269,7 @@
     </row>
     <row r="52" spans="7:7">
       <c r="G52" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="53" spans="7:7">
@@ -6276,17 +6279,17 @@
     </row>
     <row r="54" spans="7:7">
       <c r="G54" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="55" spans="7:7">
       <c r="G55" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="56" spans="7:7">
       <c r="G56" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="57" spans="7:7">
@@ -6296,7 +6299,7 @@
     </row>
     <row r="58" spans="7:7">
       <c r="G58" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="59" spans="7:7">
@@ -6306,7 +6309,7 @@
     </row>
     <row r="60" spans="7:7">
       <c r="G60" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="61" spans="7:7">
@@ -6316,7 +6319,7 @@
     </row>
     <row r="62" spans="7:7">
       <c r="G62" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="63" spans="7:7">
@@ -6336,12 +6339,12 @@
     </row>
     <row r="66" spans="7:7">
       <c r="G66" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="67" spans="7:7">
       <c r="G67" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="68" spans="7:7">
@@ -6371,7 +6374,7 @@
     </row>
     <row r="73" spans="7:7">
       <c r="G73" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
   </sheetData>
@@ -6381,1538 +6384,1661 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A305"/>
+  <dimension ref="A1:F305"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="E1">
+        <v>124</v>
+      </c>
+      <c r="F1" t="str">
+        <f>INDEX(A:A, E1, 1)</f>
+        <v>ham</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2">
+        <v>92</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f t="shared" ref="F2:F15" si="0">INDEX(A:A, E2, 1)</f>
+        <v>drpepper</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3">
+        <v>304</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>ziploc_bag</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>astro_yogurt</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>boneless_pork_chop</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="1" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>balderson_cheese</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="1" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7">
+        <v>116</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>grape</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="1" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8">
+        <v>60</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>cling_wrap</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="1" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9">
+        <v>141</v>
+      </c>
+      <c r="F9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>johnson's</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="1" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <v>51</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>cheese_bar</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="1" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11">
+        <v>195</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pc_chicken_breast</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="1" t="s">
+      <c r="D12" s="1"/>
+      <c r="E12">
+        <v>98</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>entree</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="1" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13">
+        <v>145</v>
+      </c>
+      <c r="F13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>kebab</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="1" t="s">
+      <c r="D14" s="1"/>
+      <c r="E14">
+        <v>242</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>salsa</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="1" t="s">
+      <c r="D15" s="1"/>
+      <c r="E15">
+        <v>127</v>
+      </c>
+      <c r="F15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>head&amp;shoulders_shampoo</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
         <v>604</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="1" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="1" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="1" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="1" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="1" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="1" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="1" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="1" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="1" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="1" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="1" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="1" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="1" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="1" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="1" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="1" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="1" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="1" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="1" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="1" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="1" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="1" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="1" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="1" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="1" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="1" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="1" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="1" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="1" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="1" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="1" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="1" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="1" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="1" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="1" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="1" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="1" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="1" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="1" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="1" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="1" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="1" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="1" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="1" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="1" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="1" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="1" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="1" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="1" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="1" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="1" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="1" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="1" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="1" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="1" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="1" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="1" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="1" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="1" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="1" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="1" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" s="1" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="1" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="1" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="1" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="1" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="1" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="1" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="1" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="1" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" s="1" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="1" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" s="1" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="1" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" s="1" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="1" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" s="1" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" s="1" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" s="1" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" s="1" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" s="1" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" s="1" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" s="1" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" s="1" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" s="1" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" s="1" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" s="1" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" s="1" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" s="1" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" s="1" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" s="1" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" s="1" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" s="1" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" s="1" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" s="1" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" s="1" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" s="1" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" s="1" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" s="1" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" s="1" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" s="1" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" s="1" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" s="1" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" s="1" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" s="1" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" s="1" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" s="1" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" s="1" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" s="1" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" s="1" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" s="1" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" s="1" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" s="1" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" s="1" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" s="1" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" s="1" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" s="1" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" s="1" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" s="1" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" s="1" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" s="1" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" s="1" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" s="1" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" s="1" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" s="1" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" s="1" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" s="1" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" s="1" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" s="1" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" s="1" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" s="1" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" s="1" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" s="1" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" s="1" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" s="1" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" s="1" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" s="1" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" s="1" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" s="1" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" s="1" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" s="1" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" s="1" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" s="1" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" s="1" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" s="1" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" s="1" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" s="1" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" s="1" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" s="1" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" s="1" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" s="1" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" s="1" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" s="1" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" s="1" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" s="1" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" s="1" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" s="1" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" s="1" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" s="1" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" s="1" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" s="1" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" s="1" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" s="1" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" s="1" t="s">
-        <v>794</v>
+        <v>897</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" s="1" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" s="1" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" s="1" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" s="1" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" s="1" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" s="1" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" s="1" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" s="1" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" s="1" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" s="1" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" s="1" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" s="1" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" s="1" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" s="1" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" s="1" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" s="1" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" s="1" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" s="1" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" s="1" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" s="1" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" s="1" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" s="1" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" s="1" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" s="1" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" s="1" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" s="1" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" s="1" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" s="1" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" s="1" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" s="1" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" s="1" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" s="1" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" s="1" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" s="1" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" s="1" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" s="1" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" s="1" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" s="1" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" s="1" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" s="1" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" s="1" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" s="1" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" s="1" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" s="1" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" s="1" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" s="1" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" s="1" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251" s="1" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252" s="1" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" s="1" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" s="1" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" s="1" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" s="1" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" s="1" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" s="1" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" s="1" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" s="1" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261" s="1" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262" s="1" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" s="1" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" s="1" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" s="1" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" s="1" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" s="1" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" s="1" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" s="1" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" s="1" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" s="1" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" s="1" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" s="1" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" s="1" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" s="1" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" s="1" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" s="1" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" s="1" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" s="1" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" s="1" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" s="1" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" s="1" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" s="1" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" s="1" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" s="1" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" s="1" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" s="1" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" s="1" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" s="1" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" s="1" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" s="1" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" s="1" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" s="1" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" s="1" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" s="1" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" s="1" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" s="1" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" s="1" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" s="1" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" s="1" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" s="1" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" s="1" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" s="1" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" s="1" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" s="1" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed the apostrophe issue in excel sheet
</commit_message>
<xml_diff>
--- a/RandomData/inventory.xlsx
+++ b/RandomData/inventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11760" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="zehrs" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="897">
   <si>
     <t>coca_cola 350</t>
   </si>
@@ -678,9 +678,6 @@
     <t>energy_bar 149</t>
   </si>
   <si>
-    <t>uncle_ben’s 800</t>
-  </si>
-  <si>
     <t>cooking_spray 449</t>
   </si>
   <si>
@@ -2652,9 +2649,6 @@
     <t>twizzler</t>
   </si>
   <si>
-    <t>uncle_ben’s</t>
-  </si>
-  <si>
     <t>uncle_ben's</t>
   </si>
   <si>
@@ -2716,6 +2710,9 @@
   </si>
   <si>
     <t>peach</t>
+  </si>
+  <si>
+    <t>uncle_ben's 800</t>
   </si>
 </sst>
 </file>
@@ -3018,7 +3015,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3028,8 +3025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="E1:E161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="F129" sqref="F129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3049,12 +3046,12 @@
     </row>
     <row r="3" spans="5:5">
       <c r="E3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="5:5">
       <c r="E4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="5" spans="5:5">
@@ -3064,12 +3061,12 @@
     </row>
     <row r="6" spans="5:5">
       <c r="E6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="5:5">
       <c r="E7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="8" spans="5:5">
@@ -3084,7 +3081,7 @@
     </row>
     <row r="10" spans="5:5">
       <c r="E10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="5:5">
@@ -3109,7 +3106,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="16" spans="5:5">
@@ -3124,7 +3121,7 @@
     </row>
     <row r="18" spans="5:5">
       <c r="E18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="5:5">
@@ -3144,7 +3141,7 @@
     </row>
     <row r="22" spans="5:5">
       <c r="E22" s="1" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="23" spans="5:5">
@@ -3154,7 +3151,7 @@
     </row>
     <row r="24" spans="5:5">
       <c r="E24" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="25" spans="5:5">
@@ -3164,7 +3161,7 @@
     </row>
     <row r="26" spans="5:5">
       <c r="E26" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="27" spans="5:5">
@@ -3174,7 +3171,7 @@
     </row>
     <row r="28" spans="5:5">
       <c r="E28" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="29" spans="5:5">
@@ -3184,7 +3181,7 @@
     </row>
     <row r="30" spans="5:5">
       <c r="E30" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="31" spans="5:5">
@@ -3194,7 +3191,7 @@
     </row>
     <row r="32" spans="5:5">
       <c r="E32" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="33" spans="5:5">
@@ -3244,12 +3241,12 @@
     </row>
     <row r="42" spans="5:5">
       <c r="E42" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="43" spans="5:5">
       <c r="E43" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="44" spans="5:5">
@@ -3279,7 +3276,7 @@
     </row>
     <row r="49" spans="5:5">
       <c r="E49" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="50" spans="5:5">
@@ -3289,22 +3286,22 @@
     </row>
     <row r="51" spans="5:5">
       <c r="E51" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="52" spans="5:5">
       <c r="E52" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="53" spans="5:5">
       <c r="E53" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="54" spans="5:5">
       <c r="E54" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="55" spans="5:5">
@@ -3329,7 +3326,7 @@
     </row>
     <row r="59" spans="5:5">
       <c r="E59" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="60" spans="5:5">
@@ -3339,7 +3336,7 @@
     </row>
     <row r="61" spans="5:5">
       <c r="E61" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="62" spans="5:5">
@@ -3349,22 +3346,22 @@
     </row>
     <row r="63" spans="5:5">
       <c r="E63" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="64" spans="5:5">
       <c r="E64" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="65" spans="5:5">
       <c r="E65" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="66" spans="5:5">
       <c r="E66" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="67" spans="5:5">
@@ -3384,7 +3381,7 @@
     </row>
     <row r="70" spans="5:5">
       <c r="E70" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="71" spans="5:5">
@@ -3394,12 +3391,12 @@
     </row>
     <row r="72" spans="5:5">
       <c r="E72" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="73" spans="5:5">
       <c r="E73" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="74" spans="5:5">
@@ -3414,7 +3411,7 @@
     </row>
     <row r="76" spans="5:5">
       <c r="E76" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="77" spans="5:5">
@@ -3429,7 +3426,7 @@
     </row>
     <row r="79" spans="5:5">
       <c r="E79" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="80" spans="5:5">
@@ -3439,42 +3436,42 @@
     </row>
     <row r="81" spans="5:5">
       <c r="E81" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="89" spans="5:5">
@@ -3484,7 +3481,7 @@
     </row>
     <row r="90" spans="5:5">
       <c r="E90" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="91" spans="5:5">
@@ -3494,7 +3491,7 @@
     </row>
     <row r="92" spans="5:5">
       <c r="E92" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="93" spans="5:5">
@@ -3504,7 +3501,7 @@
     </row>
     <row r="94" spans="5:5">
       <c r="E94" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="95" spans="5:5">
@@ -3519,17 +3516,17 @@
     </row>
     <row r="97" spans="5:5">
       <c r="E97" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="99" spans="5:5">
       <c r="E99" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="100" spans="5:5">
@@ -3539,22 +3536,22 @@
     </row>
     <row r="101" spans="5:5">
       <c r="E101" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="102" spans="5:5">
       <c r="E102" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="103" spans="5:5">
       <c r="E103" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="104" spans="5:5">
       <c r="E104" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="105" spans="5:5">
@@ -3579,7 +3576,7 @@
     </row>
     <row r="109" spans="5:5">
       <c r="E109" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="110" spans="5:5">
@@ -3589,12 +3586,12 @@
     </row>
     <row r="111" spans="5:5">
       <c r="E111" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="112" spans="5:5">
       <c r="E112" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="113" spans="5:5">
@@ -3624,7 +3621,7 @@
     </row>
     <row r="118" spans="5:5">
       <c r="E118" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="119" spans="5:5">
@@ -3634,7 +3631,7 @@
     </row>
     <row r="120" spans="5:5">
       <c r="E120" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="121" spans="5:5">
@@ -3644,7 +3641,7 @@
     </row>
     <row r="122" spans="5:5">
       <c r="E122" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="123" spans="5:5">
@@ -3654,7 +3651,7 @@
     </row>
     <row r="124" spans="5:5">
       <c r="E124" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="125" spans="5:5">
@@ -3664,37 +3661,37 @@
     </row>
     <row r="126" spans="5:5">
       <c r="E126" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="127" spans="5:5">
       <c r="E127" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="128" spans="5:5">
       <c r="E128" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="129" spans="5:5">
       <c r="E129" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="130" spans="5:5">
       <c r="E130" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="131" spans="5:5">
       <c r="E131" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="132" spans="5:5">
       <c r="E132" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="133" spans="5:5">
@@ -3714,12 +3711,12 @@
     </row>
     <row r="136" spans="5:5">
       <c r="E136" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="137" spans="5:5">
       <c r="E137" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="138" spans="5:5">
@@ -3749,17 +3746,17 @@
     </row>
     <row r="143" spans="5:5">
       <c r="E143" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="144" spans="5:5">
       <c r="E144" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="145" spans="5:5">
       <c r="E145" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="146" spans="5:5">
@@ -3769,7 +3766,7 @@
     </row>
     <row r="147" spans="5:5">
       <c r="E147" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="148" spans="5:5">
@@ -3789,12 +3786,12 @@
     </row>
     <row r="151" spans="5:5">
       <c r="E151" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="152" spans="5:5">
       <c r="E152" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="153" spans="5:5">
@@ -3809,27 +3806,27 @@
     </row>
     <row r="155" spans="5:5">
       <c r="E155" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="156" spans="5:5">
       <c r="E156" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="157" spans="5:5">
       <c r="E157" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="158" spans="5:5">
       <c r="E158" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="159" spans="5:5">
       <c r="E159" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="160" spans="5:5">
@@ -3859,27 +3856,27 @@
   <sheetData>
     <row r="1" spans="5:5">
       <c r="E1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="2" spans="5:5">
       <c r="E2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3" spans="5:5">
       <c r="E3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="4" spans="5:5">
       <c r="E4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5" spans="5:5">
       <c r="E5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="6" spans="5:5">
@@ -3889,7 +3886,7 @@
     </row>
     <row r="7" spans="5:5">
       <c r="E7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="8" spans="5:5">
@@ -3904,12 +3901,12 @@
     </row>
     <row r="10" spans="5:5">
       <c r="E10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="11" spans="5:5">
       <c r="E11" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="12" spans="5:5">
@@ -3919,7 +3916,7 @@
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -3929,7 +3926,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="16" spans="5:5">
@@ -3939,7 +3936,7 @@
     </row>
     <row r="17" spans="5:5">
       <c r="E17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="18" spans="5:5">
@@ -3949,7 +3946,7 @@
     </row>
     <row r="19" spans="5:5">
       <c r="E19" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="20" spans="5:5">
@@ -3959,12 +3956,12 @@
     </row>
     <row r="21" spans="5:5">
       <c r="E21" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="22" spans="5:5">
       <c r="E22" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="23" spans="5:5">
@@ -3984,22 +3981,22 @@
     </row>
     <row r="26" spans="5:5">
       <c r="E26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="27" spans="5:5">
       <c r="E27" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="28" spans="5:5">
       <c r="E28" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="29" spans="5:5">
       <c r="E29" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="30" spans="5:5">
@@ -4019,7 +4016,7 @@
     </row>
     <row r="33" spans="5:5">
       <c r="E33" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="34" spans="5:5">
@@ -4074,7 +4071,7 @@
     </row>
     <row r="44" spans="5:5">
       <c r="E44" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="45" spans="5:5">
@@ -4084,12 +4081,12 @@
     </row>
     <row r="46" spans="5:5">
       <c r="E46" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="47" spans="5:5">
       <c r="E47" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="48" spans="5:5">
@@ -4099,7 +4096,7 @@
     </row>
     <row r="49" spans="5:5">
       <c r="E49" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="50" spans="5:5">
@@ -4114,7 +4111,7 @@
     </row>
     <row r="52" spans="5:5">
       <c r="E52" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="53" spans="5:5">
@@ -4129,7 +4126,7 @@
     </row>
     <row r="55" spans="5:5">
       <c r="E55" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
   </sheetData>
@@ -4164,7 +4161,7 @@
     </row>
     <row r="4" spans="4:4">
       <c r="D4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" spans="4:4">
@@ -4189,27 +4186,27 @@
     </row>
     <row r="9" spans="4:4">
       <c r="D9" s="1" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
     </row>
     <row r="10" spans="4:4">
       <c r="D10" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="11" spans="4:4">
       <c r="D11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="12" spans="4:4">
       <c r="D12" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="13" spans="4:4">
       <c r="D13" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="14" spans="4:4">
@@ -4219,7 +4216,7 @@
     </row>
     <row r="15" spans="4:4">
       <c r="D15" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="16" spans="4:4">
@@ -4229,22 +4226,22 @@
     </row>
     <row r="17" spans="4:4">
       <c r="D17" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="18" spans="4:4">
       <c r="D18" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="19" spans="4:4">
       <c r="D19" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="20" spans="4:4">
       <c r="D20" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="21" spans="4:4">
@@ -4269,12 +4266,12 @@
     </row>
     <row r="25" spans="4:4">
       <c r="D25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="26" spans="4:4">
       <c r="D26" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="27" spans="4:4">
@@ -4299,12 +4296,12 @@
     </row>
     <row r="31" spans="4:4">
       <c r="D31" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="32" spans="4:4">
       <c r="D32" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="33" spans="4:4">
@@ -4314,7 +4311,7 @@
     </row>
     <row r="34" spans="4:4">
       <c r="D34" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="35" spans="4:4">
@@ -4344,7 +4341,7 @@
     </row>
     <row r="40" spans="4:4">
       <c r="D40" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="41" spans="4:4">
@@ -4354,22 +4351,22 @@
     </row>
     <row r="42" spans="4:4">
       <c r="D42" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="43" spans="4:4">
       <c r="D43" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="44" spans="4:4">
       <c r="D44" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="45" spans="4:4">
       <c r="D45" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="46" spans="4:4">
@@ -4379,27 +4376,27 @@
     </row>
     <row r="47" spans="4:4">
       <c r="D47" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="48" spans="4:4">
       <c r="D48" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="49" spans="4:4">
       <c r="D49" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="50" spans="4:4">
       <c r="D50" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="51" spans="4:4">
       <c r="D51" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="52" spans="4:4">
@@ -4414,7 +4411,7 @@
     </row>
     <row r="54" spans="4:4">
       <c r="D54" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="55" spans="4:4">
@@ -4429,7 +4426,7 @@
     </row>
     <row r="57" spans="4:4">
       <c r="D57" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="58" spans="4:4">
@@ -4439,7 +4436,7 @@
     </row>
     <row r="59" spans="4:4">
       <c r="D59" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="60" spans="4:4">
@@ -4454,12 +4451,12 @@
     </row>
     <row r="62" spans="4:4">
       <c r="D62" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="63" spans="4:4">
       <c r="D63" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="64" spans="4:4">
@@ -4479,12 +4476,12 @@
     </row>
     <row r="67" spans="4:4">
       <c r="D67" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="68" spans="4:4">
       <c r="D68" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="69" spans="4:4">
@@ -4499,12 +4496,12 @@
     </row>
     <row r="71" spans="4:4">
       <c r="D71" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="72" spans="4:4">
       <c r="D72" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="73" spans="4:4">
@@ -4534,12 +4531,12 @@
     </row>
     <row r="78" spans="4:4">
       <c r="D78" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="79" spans="4:4">
       <c r="D79" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="80" spans="4:4">
@@ -4564,7 +4561,7 @@
     </row>
     <row r="84" spans="4:4">
       <c r="D84" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="85" spans="4:4">
@@ -4594,12 +4591,12 @@
     </row>
     <row r="90" spans="4:4">
       <c r="D90" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="91" spans="4:4">
       <c r="D91" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="92" spans="4:4">
@@ -4639,7 +4636,7 @@
     </row>
     <row r="99" spans="4:4">
       <c r="D99" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="100" spans="4:4">
@@ -4656,8 +4653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="E1:E98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4669,7 +4666,7 @@
     </row>
     <row r="2" spans="5:5">
       <c r="E2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" spans="5:5">
@@ -4684,12 +4681,12 @@
     </row>
     <row r="5" spans="5:5">
       <c r="E5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="6" spans="5:5">
       <c r="E6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="7" spans="5:5">
@@ -4709,7 +4706,7 @@
     </row>
     <row r="10" spans="5:5">
       <c r="E10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="11" spans="5:5">
@@ -4719,12 +4716,12 @@
     </row>
     <row r="12" spans="5:5">
       <c r="E12" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -4769,17 +4766,17 @@
     </row>
     <row r="22" spans="5:5">
       <c r="E22" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="23" spans="5:5">
       <c r="E23" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="24" spans="5:5">
       <c r="E24" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="25" spans="5:5">
@@ -4819,7 +4816,7 @@
     </row>
     <row r="32" spans="5:5">
       <c r="E32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="33" spans="5:5">
@@ -4839,7 +4836,7 @@
     </row>
     <row r="36" spans="5:5">
       <c r="E36" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="37" spans="5:5">
@@ -4949,22 +4946,22 @@
     </row>
     <row r="58" spans="5:5">
       <c r="E58" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="59" spans="5:5">
       <c r="E59" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="60" spans="5:5">
       <c r="E60" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="61" spans="5:5">
       <c r="E61" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="62" spans="5:5">
@@ -4974,152 +4971,152 @@
     </row>
     <row r="63" spans="5:5">
       <c r="E63" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="64" spans="5:5">
-      <c r="E64" t="s">
-        <v>218</v>
+      <c r="E64" s="1" t="s">
+        <v>896</v>
       </c>
     </row>
     <row r="65" spans="5:5">
       <c r="E65" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="66" spans="5:5">
       <c r="E66" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="67" spans="5:5">
       <c r="E67" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="68" spans="5:5">
       <c r="E68" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="69" spans="5:5">
       <c r="E69" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="70" spans="5:5">
       <c r="E70" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="71" spans="5:5">
       <c r="E71" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="72" spans="5:5">
       <c r="E72" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="73" spans="5:5">
       <c r="E73" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="74" spans="5:5">
       <c r="E74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="75" spans="5:5">
       <c r="E75" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="76" spans="5:5">
       <c r="E76" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="77" spans="5:5">
       <c r="E77" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="78" spans="5:5">
       <c r="E78" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="79" spans="5:5">
       <c r="E79" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80" spans="5:5">
       <c r="E80" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="81" spans="5:5">
       <c r="E81" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="82" spans="5:5">
       <c r="E82" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="83" spans="5:5">
       <c r="E83" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="84" spans="5:5">
       <c r="E84" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="85" spans="5:5">
       <c r="E85" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="86" spans="5:5">
       <c r="E86" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="87" spans="5:5">
       <c r="E87" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="88" spans="5:5">
       <c r="E88" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="89" spans="5:5">
       <c r="E89" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="90" spans="5:5">
       <c r="E90" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="91" spans="5:5">
       <c r="E91" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="92" spans="5:5">
       <c r="E92" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="93" spans="5:5">
@@ -5129,12 +5126,12 @@
     </row>
     <row r="94" spans="5:5">
       <c r="E94" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="95" spans="5:5">
       <c r="E95" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="96" spans="5:5">
@@ -5144,12 +5141,12 @@
     </row>
     <row r="97" spans="5:5">
       <c r="E97" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="98" spans="5:5">
       <c r="E98" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -5169,147 +5166,147 @@
   <sheetData>
     <row r="1" spans="5:5">
       <c r="E1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="2" spans="5:5">
       <c r="E2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="5:5">
       <c r="E3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="5:5">
       <c r="E4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="5" spans="5:5">
       <c r="E5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="6" spans="5:5">
       <c r="E6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="5:5">
       <c r="E7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="5:5">
       <c r="E8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="5:5">
       <c r="E9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="5:5">
       <c r="E10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="5:5">
       <c r="E11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="5:5">
       <c r="E12" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="5:5">
       <c r="E14" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="16" spans="5:5">
       <c r="E16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="5:5">
       <c r="E17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="5:5">
       <c r="E18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="5:5">
       <c r="E19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="5:5">
       <c r="E20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="5:5">
       <c r="E21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="5:5">
       <c r="E22" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="23" spans="5:5">
       <c r="E23" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="24" spans="5:5">
       <c r="E24" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="25" spans="5:5">
       <c r="E25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="5:5">
       <c r="E26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="5:5">
       <c r="E27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="5:5">
       <c r="E28" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="29" spans="5:5">
       <c r="E29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -5321,15 +5318,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="E1:E78"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="5:5">
       <c r="E1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="5:5">
@@ -5339,7 +5336,7 @@
     </row>
     <row r="3" spans="5:5">
       <c r="E3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="5:5">
@@ -5349,12 +5346,12 @@
     </row>
     <row r="5" spans="5:5">
       <c r="E5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="6" spans="5:5">
       <c r="E6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="5:5">
@@ -5364,7 +5361,7 @@
     </row>
     <row r="8" spans="5:5">
       <c r="E8" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="9" spans="5:5">
@@ -5379,7 +5376,7 @@
     </row>
     <row r="11" spans="5:5">
       <c r="E11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="5:5">
@@ -5389,12 +5386,12 @@
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="14" spans="5:5">
       <c r="E14" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="15" spans="5:5">
@@ -5404,17 +5401,17 @@
     </row>
     <row r="16" spans="5:5">
       <c r="E16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="5:5">
       <c r="E17" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="18" spans="5:5">
       <c r="E18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="19" spans="5:5">
@@ -5434,22 +5431,22 @@
     </row>
     <row r="22" spans="5:5">
       <c r="E22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="23" spans="5:5">
       <c r="E23" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="24" spans="5:5">
       <c r="E24" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="25" spans="5:5">
       <c r="E25" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="26" spans="5:5">
@@ -5459,17 +5456,17 @@
     </row>
     <row r="27" spans="5:5">
       <c r="E27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" spans="5:5">
       <c r="E28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29" spans="5:5">
       <c r="E29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="5:5">
@@ -5479,32 +5476,32 @@
     </row>
     <row r="31" spans="5:5">
       <c r="E31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="32" spans="5:5">
       <c r="E32" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="33" spans="5:5">
       <c r="E33" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="34" spans="5:5">
       <c r="E34" s="1" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="35" spans="5:5">
       <c r="E35" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="36" spans="5:5">
       <c r="E36" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="37" spans="5:5">
@@ -5514,27 +5511,27 @@
     </row>
     <row r="38" spans="5:5">
       <c r="E38" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="39" spans="5:5">
       <c r="E39" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="40" spans="5:5">
       <c r="E40" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="41" spans="5:5">
       <c r="E41" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="42" spans="5:5">
       <c r="E42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="43" spans="5:5">
@@ -5544,57 +5541,57 @@
     </row>
     <row r="44" spans="5:5">
       <c r="E44" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="45" spans="5:5">
       <c r="E45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="46" spans="5:5">
       <c r="E46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="47" spans="5:5">
       <c r="E47" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="48" spans="5:5">
       <c r="E48" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" spans="5:5">
       <c r="E49" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="50" spans="5:5">
       <c r="E50" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="51" spans="5:5">
       <c r="E51" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="5:5">
       <c r="E52" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="53" spans="5:5">
       <c r="E53" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="54" spans="5:5">
       <c r="E54" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="55" spans="5:5">
@@ -5604,102 +5601,102 @@
     </row>
     <row r="56" spans="5:5">
       <c r="E56" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="57" spans="5:5">
       <c r="E57" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="58" spans="5:5">
       <c r="E58" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="59" spans="5:5">
       <c r="E59" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="60" spans="5:5">
       <c r="E60" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="61" spans="5:5">
       <c r="E61" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="62" spans="5:5">
       <c r="E62" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="63" spans="5:5">
       <c r="E63" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="64" spans="5:5">
       <c r="E64" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="65" spans="5:5">
       <c r="E65" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="66" spans="5:5">
       <c r="E66" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="67" spans="5:5">
       <c r="E67" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="68" spans="5:5">
       <c r="E68" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="69" spans="5:5">
       <c r="E69" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="70" spans="5:5">
       <c r="E70" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="71" spans="5:5">
       <c r="E71" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="72" spans="5:5">
       <c r="E72" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="73" spans="5:5">
       <c r="E73" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="74" spans="5:5">
       <c r="E74" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="75" spans="5:5">
       <c r="E75" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="76" spans="5:5">
@@ -5709,12 +5706,12 @@
     </row>
     <row r="77" spans="5:5">
       <c r="E77" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="78" spans="5:5">
       <c r="E78" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -5734,222 +5731,222 @@
   <sheetData>
     <row r="1" spans="7:7">
       <c r="G1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" spans="7:7">
       <c r="G2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="7:7">
       <c r="G3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="7:7">
       <c r="G4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="7:7">
       <c r="G5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="7:7">
       <c r="G6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="7:7">
       <c r="G7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="7:7">
       <c r="G8" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="9" spans="7:7">
       <c r="G9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10" spans="7:7">
       <c r="G10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="11" spans="7:7">
       <c r="G11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="12" spans="7:7">
       <c r="G12" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="13" spans="7:7">
       <c r="G13" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="14" spans="7:7">
       <c r="G14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="15" spans="7:7">
       <c r="G15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="16" spans="7:7">
       <c r="G16" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="7:7">
       <c r="G17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" spans="7:7">
       <c r="G18" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="19" spans="7:7">
       <c r="G19" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="20" spans="7:7">
       <c r="G20" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="21" spans="7:7">
       <c r="G21" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="22" spans="7:7">
       <c r="G22" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="23" spans="7:7">
       <c r="G23" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="24" spans="7:7">
       <c r="G24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="25" spans="7:7">
       <c r="G25" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="26" spans="7:7">
       <c r="G26" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="27" spans="7:7">
       <c r="G27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="28" spans="7:7">
       <c r="G28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="29" spans="7:7">
       <c r="G29" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="30" spans="7:7">
       <c r="G30" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="31" spans="7:7">
       <c r="G31" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="32" spans="7:7">
       <c r="G32" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="33" spans="7:7">
       <c r="G33" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="34" spans="7:7">
       <c r="G34" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="35" spans="7:7">
       <c r="G35" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="36" spans="7:7">
       <c r="G36" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="37" spans="7:7">
       <c r="G37" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="38" spans="7:7">
       <c r="G38" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="39" spans="7:7">
       <c r="G39" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="40" spans="7:7">
       <c r="G40" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="41" spans="7:7">
       <c r="G41" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="42" spans="7:7">
       <c r="G42" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="43" spans="7:7">
       <c r="G43" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="44" spans="7:7">
       <c r="G44" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="45" spans="7:7">
@@ -5959,42 +5956,42 @@
     </row>
     <row r="46" spans="7:7">
       <c r="G46" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="47" spans="7:7">
       <c r="G47" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="48" spans="7:7">
       <c r="G48" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="49" spans="7:7">
       <c r="G49" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="50" spans="7:7">
       <c r="G50" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="51" spans="7:7">
       <c r="G51" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="52" spans="7:7">
       <c r="G52" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="53" spans="7:7">
       <c r="G53" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -6014,117 +6011,117 @@
   <sheetData>
     <row r="1" spans="7:7">
       <c r="G1" s="1" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
     <row r="2" spans="7:7">
       <c r="G2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="7:7">
       <c r="G3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="7:7">
       <c r="G4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="7:7">
       <c r="G5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="6" spans="7:7">
       <c r="G6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="7:7">
       <c r="G7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="7:7">
       <c r="G8" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="9" spans="7:7">
       <c r="G9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="10" spans="7:7">
       <c r="G10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="11" spans="7:7">
       <c r="G11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="12" spans="7:7">
       <c r="G12" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="13" spans="7:7">
       <c r="G13" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="14" spans="7:7">
       <c r="G14" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="15" spans="7:7">
       <c r="G15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="7:7">
       <c r="G16" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="17" spans="7:7">
       <c r="G17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="18" spans="7:7">
       <c r="G18" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="19" spans="7:7">
       <c r="G19" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="20" spans="7:7">
       <c r="G20" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="21" spans="7:7">
       <c r="G21" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="22" spans="7:7">
       <c r="G22" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="23" spans="7:7">
       <c r="G23" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24" spans="7:7">
@@ -6134,27 +6131,27 @@
     </row>
     <row r="25" spans="7:7">
       <c r="G25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="26" spans="7:7">
       <c r="G26" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="27" spans="7:7">
       <c r="G27" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="28" spans="7:7">
       <c r="G28" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="29" spans="7:7">
       <c r="G29" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="30" spans="7:7">
@@ -6164,32 +6161,32 @@
     </row>
     <row r="31" spans="7:7">
       <c r="G31" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="32" spans="7:7">
       <c r="G32" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="33" spans="7:7">
       <c r="G33" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="34" spans="7:7">
       <c r="G34" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="35" spans="7:7">
       <c r="G35" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="36" spans="7:7">
       <c r="G36" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="37" spans="7:7">
@@ -6199,182 +6196,182 @@
     </row>
     <row r="38" spans="7:7">
       <c r="G38" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="39" spans="7:7">
       <c r="G39" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" spans="7:7">
       <c r="G40" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="41" spans="7:7">
       <c r="G41" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="42" spans="7:7">
       <c r="G42" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="43" spans="7:7">
       <c r="G43" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="44" spans="7:7">
       <c r="G44" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="45" spans="7:7">
       <c r="G45" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="46" spans="7:7">
       <c r="G46" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="47" spans="7:7">
       <c r="G47" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="48" spans="7:7">
       <c r="G48" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="49" spans="7:7">
       <c r="G49" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="50" spans="7:7">
       <c r="G50" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="51" spans="7:7">
       <c r="G51" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="52" spans="7:7">
       <c r="G52" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="53" spans="7:7">
       <c r="G53" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="54" spans="7:7">
       <c r="G54" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="55" spans="7:7">
       <c r="G55" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="56" spans="7:7">
       <c r="G56" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="57" spans="7:7">
       <c r="G57" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="58" spans="7:7">
       <c r="G58" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="59" spans="7:7">
       <c r="G59" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="60" spans="7:7">
       <c r="G60" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="61" spans="7:7">
       <c r="G61" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="62" spans="7:7">
       <c r="G62" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="63" spans="7:7">
       <c r="G63" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="64" spans="7:7">
       <c r="G64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="65" spans="7:7">
       <c r="G65" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="66" spans="7:7">
       <c r="G66" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="67" spans="7:7">
       <c r="G67" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="68" spans="7:7">
       <c r="G68" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="69" spans="7:7">
       <c r="G69" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="70" spans="7:7">
       <c r="G70" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="71" spans="7:7">
       <c r="G71" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="72" spans="7:7">
       <c r="G72" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="73" spans="7:7">
       <c r="G73" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
   </sheetData>
@@ -6384,9 +6381,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F305"/>
+  <dimension ref="A1:F304"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A268" workbookViewId="0">
+      <selection activeCell="A289" sqref="A289"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -6396,10 +6395,10 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E1">
         <v>124</v>
@@ -6411,1634 +6410,1629 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2">
         <v>92</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f t="shared" ref="F2:F15" si="0">INDEX(A:A, E2, 1)</f>
+        <f>INDEX(A:A, E2, 1)</f>
         <v>drpepper</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3">
         <v>304</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>ziploc_bag</v>
+        <f>INDEX(A:A, E3, 1)</f>
+        <v>zucchini</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>INDEX(A:A, E4, 1)</f>
         <v>astro_yogurt</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5">
         <v>32</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>INDEX(A:A, E5, 1)</f>
         <v>boneless_pork_chop</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6">
         <v>19</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>INDEX(A:A, E6, 1)</f>
         <v>balderson_cheese</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7">
         <v>116</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>INDEX(A:A, E7, 1)</f>
         <v>grape</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8">
         <v>60</v>
       </c>
       <c r="F8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>INDEX(A:A, E8, 1)</f>
         <v>cling_wrap</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9">
         <v>141</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>INDEX(A:A, E9, 1)</f>
         <v>johnson's</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10">
         <v>51</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>INDEX(A:A, E10, 1)</f>
         <v>cheese_bar</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11">
         <v>195</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>INDEX(A:A, E11, 1)</f>
         <v>pc_chicken_breast</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12">
         <v>98</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>INDEX(A:A, E12, 1)</f>
         <v>entree</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13">
         <v>145</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>INDEX(A:A, E13, 1)</f>
         <v>kebab</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14">
         <v>242</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>INDEX(A:A, E14, 1)</f>
         <v>salsa</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15">
         <v>127</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>INDEX(A:A, E15, 1)</f>
         <v>head&amp;shoulders_shampoo</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" s="1" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" s="1" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" s="1" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" s="1" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" s="1" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" s="1" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" s="1" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" s="1" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" s="1" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" s="1" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" s="1" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" s="1" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" s="1" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" s="1" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" s="1" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" s="1" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" s="1" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" s="1" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" s="1" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" s="1" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" s="1" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" s="1" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" s="1" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" s="1" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" s="1" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" s="1" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" s="1" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" s="1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" s="1" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" s="1" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" s="1" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" s="1" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" s="1" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" s="1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" s="1" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" s="1" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" s="1" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" s="1" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" s="1" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" s="1" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" s="1" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" s="1" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" s="1" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" s="1" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" s="1" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" s="1" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" s="1" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" s="1" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" s="1" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" s="1" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" s="1" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" s="1" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" s="1" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" s="1" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" s="1" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" s="1" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" s="1" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" s="1" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" s="1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" s="1" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" s="1" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" s="1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" s="1" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251" s="1" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252" s="1" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" s="1" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262" s="1" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" s="1" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" s="1" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" s="1" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" s="1" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" s="1" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" s="1" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" s="1" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" s="1" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" s="1" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" s="1" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" s="1" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" s="1" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" s="1" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" s="1" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" s="1" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" s="1" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" s="1" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" s="1" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" s="1" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" s="1" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" s="1" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" s="1" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" s="1" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" s="1" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" s="1" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" s="1" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" s="1" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" s="1" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" s="1" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" s="1" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" s="1" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" s="1" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" s="1" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" s="1" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" s="1" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="305" spans="1:1">
-      <c r="A305" s="1" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>